<commit_message>
update bug fix finance & check VA & Klasifikasi Bintang
</commit_message>
<xml_diff>
--- a/document/PenerimaanPembayaran.xlsx
+++ b/document/PenerimaanPembayaran.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>YAYASAN PENDIDIKAN AGUNG PODOMORO</t>
   </si>
   <si>
-    <t>Rekap Penerimaan &amp; AGING 2018/2019 Ganjil</t>
+    <t>Rekap Penerimaan &amp; AGING 2017/2018 Genap</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -64,36 +64,6 @@
   </si>
   <si>
     <t>Ket</t>
-  </si>
-  <si>
-    <t>VENI CAHYANI</t>
-  </si>
-  <si>
-    <t>Entrepreneurship</t>
-  </si>
-  <si>
-    <t>Lunas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VANESSA BELLA PUTRI </t>
-  </si>
-  <si>
-    <t>WILLIAM</t>
-  </si>
-  <si>
-    <t>DEAN KEMILAU LIUSONO</t>
-  </si>
-  <si>
-    <t>WINDY SHANIA</t>
-  </si>
-  <si>
-    <t>AKIRA ANDERS</t>
-  </si>
-  <si>
-    <t>Belum Lunas</t>
-  </si>
-  <si>
-    <t>ALDO GINOLA</t>
   </si>
 </sst>
 </file>
@@ -245,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -290,12 +260,6 @@
     </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,10 +560,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="19.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,181 +667,6 @@
         <v>14</v>
       </c>
       <c r="K7" s="14"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="15">
-        <v>1</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="15">
-        <v>11170001</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16">
-        <v>14000000</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="15">
-        <v>2</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="15">
-        <v>11170002</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16">
-        <v>14000000</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="15">
-        <v>3</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="15">
-        <v>11160001</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16">
-        <v>0</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="15">
-        <v>4</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="15">
-        <v>11170021</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16">
-        <v>8300000</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="15">
-        <v>5</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="15">
-        <v>11170022</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16">
-        <v>8300000</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="15">
-        <v>6</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="15">
-        <v>11170019</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16">
-        <v>7000000</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="15">
-        <v>7</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="15">
-        <v>11150003</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16">
-        <v>9100000</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>